<commit_message>
#add data file-->items #debug inventory manager #debug loadtxt
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cn_Sky/newworld/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oas/Documents/work/github/newworld/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="7360" yWindow="3020" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -894,7 +897,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
#Update map, fix bugs #Debug moving
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oas/Documents/work/github/newworld/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cn_Sky/newworld/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38320" yWindow="1620" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -33,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="303">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -2514,16 +2511,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>生成地貌</t>
-    <rPh sb="0" eb="1">
-      <t>sheng'cheng</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>得出npc列表</t>
     <rPh sb="0" eb="1">
       <t>de'chu</t>
@@ -2674,332 +2661,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>大块地貌</t>
-    <rPh sb="0" eb="1">
-      <t>da'kuai</t>
+    <t>出现地貌概率</t>
+    <rPh sb="0" eb="1">
+      <t>chu'xian</t>
     </rPh>
     <rPh sb="2" eb="3">
       <t>di'mao</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>中型地貌</t>
-    <rPh sb="0" eb="1">
-      <t>zhong'xing</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>小型地貌</t>
-    <rPh sb="0" eb="1">
-      <t>xiao'xing</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>50-500格子</t>
-    <rPh sb="6" eb="7">
-      <t>ge'zi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1-10格子</t>
     <rPh sb="4" eb="5">
-      <t>ge'z</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10-50格子</t>
+      <t>gai'lv</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地貌类型概率</t>
+    <rPh sb="0" eb="1">
+      <t>di'mao'lei'xing</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>gai'lv</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图四周加边界</t>
+    <rPh sb="0" eb="1">
+      <t>di'tu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>si'zhou</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>jia</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>bian'jie</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>边界以3个格子大小为限</t>
+    <rPh sb="0" eb="1">
+      <t>bian'jie</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ge</t>
+    </rPh>
     <rPh sb="5" eb="6">
       <t>ge'zi</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地貌类型</t>
-    <rPh sb="0" eb="1">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>lei'xing</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生成规则</t>
-    <rPh sb="0" eb="1">
-      <t>shegn'chegn</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>gui'ze</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>选择初始点</t>
-    <rPh sb="0" eb="1">
-      <t>xuan'ze</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>chu'shi'dian</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确定地貌格子数</t>
-    <rPh sb="0" eb="1">
-      <t>que'ding</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>ge'zi'shu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确定行</t>
-    <rPh sb="0" eb="1">
-      <t>que'din</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>hang'lie</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>行数介于1/4~3/4格子数随机，最小为1</t>
-    <rPh sb="0" eb="1">
-      <t>hang'shu</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>jie'yu</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>ge'zi</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>zi</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>shu</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>sui'ji</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>zui'xiao</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>wei</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>确定列</t>
-    <rPh sb="0" eb="1">
-      <t>que'ding</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>lie</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>列数=格子数/行数，且向两侧随机1/5格子，最小为0</t>
-    <rPh sb="0" eb="1">
-      <t>lie</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>shu</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>ge'zi</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>shu</t>
-    </rPh>
     <rPh sb="7" eb="8">
-      <t>hang'shu</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>qie</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>xiang</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>liang'ce</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>sui'ji</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>ge'zi</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>zui'xiao</t>
-    </rPh>
-    <rPh sb="24" eb="25">
-      <t>wei</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据地貌类型，随机1-总格子数/20，有的地貌多，有的地貌少</t>
-    <rPh sb="0" eb="1">
-      <t>gen'ju</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>lei'xing</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>sui'ji</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>zong</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ge'zi</t>
-    </rPh>
-    <rPh sb="14" eb="15">
-      <t>shu</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>you</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>d</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>duo</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>you</t>
-    </rPh>
-    <rPh sb="26" eb="27">
-      <t>d</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>shao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>初始点从0,0开始，按概率触发地貌。存一个值，如果长时间不触发，值变大概率提高。如果右上方有地貌的，概率为0.</t>
-    <rPh sb="0" eb="1">
-      <t>chu'shi'dian</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>cong</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>kai'shi</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>an'gai'lv</t>
-    </rPh>
-    <rPh sb="13" eb="14">
-      <t>chu'fa</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="18" eb="19">
-      <t>cun</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>yi'ge</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>zhi</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>ru'guo</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>chang'shi'jian</t>
-    </rPh>
-    <rPh sb="28" eb="29">
-      <t>bu'chu'fa</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>chu'fa</t>
-    </rPh>
-    <rPh sb="32" eb="33">
-      <t>zhi</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>bian'da</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>gai'lv</t>
-    </rPh>
-    <rPh sb="37" eb="38">
-      <t>ti'gao</t>
-    </rPh>
-    <rPh sb="40" eb="41">
-      <t>ru'guo</t>
-    </rPh>
-    <rPh sb="42" eb="43">
-      <t>you'shang'fang</t>
-    </rPh>
-    <rPh sb="45" eb="46">
-      <t>you</t>
-    </rPh>
-    <rPh sb="46" eb="47">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="48" eb="49">
-      <t>d</t>
-    </rPh>
-    <rPh sb="50" eb="51">
-      <t>gai'lv</t>
-    </rPh>
-    <rPh sb="52" eb="53">
-      <t>wei</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>出现地貌概率</t>
-    <rPh sb="0" eb="1">
-      <t>chu'xian</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'mao</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>gai'lv</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>地貌类型概率</t>
-    <rPh sb="0" eb="1">
-      <t>di'mao'lei'xing</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>gai'lv</t>
+      <t>da'xiao</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>wei'xian</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3500,8 +3218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -3548,7 +3266,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3643,7 +3361,7 @@
         <v>282</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>316</v>
+        <v>299</v>
       </c>
       <c r="S7" t="s">
         <v>272</v>
@@ -3742,10 +3460,10 @@
         <v>281</v>
       </c>
       <c r="U9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="V9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
@@ -3791,10 +3509,10 @@
         <v>283</v>
       </c>
       <c r="U10" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="V10" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.15">
@@ -3839,13 +3557,13 @@
         <v>20,30,50,40</v>
       </c>
       <c r="T11" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U11" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="V11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.15">
@@ -3884,7 +3602,7 @@
         <v>20,30,50,40,40</v>
       </c>
       <c r="V12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.15">
@@ -3925,6 +3643,12 @@
       <c r="Q13" t="str">
         <f t="shared" si="0"/>
         <v>20,30,50,40,40,30</v>
+      </c>
+      <c r="T13" t="s">
+        <v>301</v>
+      </c>
+      <c r="U13" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.15">
@@ -4062,15 +3786,6 @@
         <f>"{"&amp;B17&amp;","&amp;C17&amp;","&amp;D17&amp;","&amp;E17&amp;","&amp;F17&amp;","&amp;G17&amp;","&amp;H17&amp;","&amp;I17&amp;","&amp;J17&amp;","&amp;K17&amp;","&amp;L17&amp;","&amp;M17&amp;","&amp;N17&amp;","&amp;O17&amp;"},"</f>
         <v>{0,1,0,0,1,0,1,0,0,1,0,0,1,1},</v>
       </c>
-      <c r="S17" t="s">
-        <v>306</v>
-      </c>
-      <c r="T17" t="s">
-        <v>300</v>
-      </c>
-      <c r="U17" t="s">
-        <v>303</v>
-      </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B18">
@@ -4133,12 +3848,6 @@
         <f t="shared" ref="P18:P24" si="3">"{"&amp;B18&amp;","&amp;C18&amp;","&amp;D18&amp;","&amp;E18&amp;","&amp;F18&amp;","&amp;G18&amp;","&amp;H18&amp;","&amp;I18&amp;","&amp;J18&amp;","&amp;K18&amp;","&amp;L18&amp;","&amp;M18&amp;","&amp;N18&amp;","&amp;O18&amp;"},"</f>
         <v>{1,1,0,0,0,1,0,0,1,1,0,0,1,1},</v>
       </c>
-      <c r="T18" t="s">
-        <v>301</v>
-      </c>
-      <c r="U18" t="s">
-        <v>305</v>
-      </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B19">
@@ -4201,12 +3910,6 @@
         <f t="shared" si="3"/>
         <v>{1,1,1,0,0,1,0,0,0,1,1,0,1,0},</v>
       </c>
-      <c r="T19" t="s">
-        <v>302</v>
-      </c>
-      <c r="U19" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B20">
@@ -4269,15 +3972,6 @@
         <f t="shared" si="3"/>
         <v>{1,1,1,0,0,1,0,0,1,1,1,0,1,0},</v>
       </c>
-      <c r="S20" t="s">
-        <v>307</v>
-      </c>
-      <c r="T20" t="s">
-        <v>308</v>
-      </c>
-      <c r="U20" t="s">
-        <v>315</v>
-      </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B21">
@@ -4340,12 +4034,6 @@
         <f t="shared" si="3"/>
         <v>{0,1,0,0,0,1,0,0,0,1,0,0,1,1},</v>
       </c>
-      <c r="T21" t="s">
-        <v>309</v>
-      </c>
-      <c r="U21" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="22" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B22">
@@ -4408,12 +4096,6 @@
         <f t="shared" si="3"/>
         <v>{0,0,1,0,0,1,0,0,1,1,0,1,1,1},</v>
       </c>
-      <c r="T22" t="s">
-        <v>310</v>
-      </c>
-      <c r="U22" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="23" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B23">
@@ -4476,12 +4158,6 @@
         <f t="shared" si="3"/>
         <v>{0,0,0,1,0,1,0,1,0,1,0,0,1,1},</v>
       </c>
-      <c r="T23" t="s">
-        <v>312</v>
-      </c>
-      <c r="U23" t="s">
-        <v>313</v>
-      </c>
     </row>
     <row r="24" spans="2:21" x14ac:dyDescent="0.15">
       <c r="B24">
@@ -4544,26 +4220,23 @@
         <f t="shared" si="3"/>
         <v>{1,0,0,0,0,0,0,0,1,1,0,0,1,1},</v>
       </c>
-      <c r="T24" t="s">
-        <v>284</v>
-      </c>
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.15">
       <c r="S28" t="s">
+        <v>285</v>
+      </c>
+      <c r="U28" t="s">
         <v>286</v>
-      </c>
-      <c r="U28" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U29" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U30" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.15">
@@ -4573,17 +4246,17 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="33" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="34" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#add landforms #add lands #add borders #debug walking
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -2700,24 +2700,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>边界以3个格子大小为限</t>
+    <t>边界=5格子</t>
     <rPh sb="0" eb="1">
       <t>bian'jie</t>
     </rPh>
-    <rPh sb="2" eb="3">
-      <t>yi</t>
-    </rPh>
     <rPh sb="4" eb="5">
-      <t>ge</t>
-    </rPh>
-    <rPh sb="5" eb="6">
       <t>ge'zi</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>da'xiao</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>wei'xian</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>

</xml_diff>

<commit_message>
#add npc #add npc model #add noctitle
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cn_Sky/newworld/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oas/Documents/work/github/newworld/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="200" yWindow="460" windowWidth="28880" windowHeight="19880" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="319">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -2706,6 +2709,118 @@
     </rPh>
     <rPh sb="4" eb="5">
       <t>ge'zi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NpcTitles</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随缘</t>
+    <rPh sb="0" eb="1">
+      <t>sui'yuan</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个油光锃亮的大和尚。</t>
+    <rPh sb="0" eb="1">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>you'guang'zeng'liang</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>d</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>da'he'shang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>随性</t>
+    <rPh sb="0" eb="1">
+      <t>sui'xing</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个衣着朴素的小和尚。</t>
+    <rPh sb="0" eb="1">
+      <t>yi'ge</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yi'zhuo'pu'su</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>d</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xiao'he'shang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hpInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atkInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>defInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>speedInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大力神僧|油面佛</t>
+    <rPh sb="0" eb="1">
+      <t>da'li'shen'seng</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>痴心和尚|飞天罗汉</t>
+    <rPh sb="0" eb="1">
+      <t>chi'xin'he'shang</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>fei'tian</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>luo'han</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nicknames</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>急速</t>
+    <rPh sb="0" eb="1">
+      <t>ji'su</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>狂躁</t>
+    <rPh sb="0" eb="1">
+      <t>kuang'zao</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2751,7 +2866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2767,6 +2882,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3206,7 +3324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
@@ -5075,10 +5193,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA42"/>
+  <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -5089,22 +5207,22 @@
     <col min="15" max="15" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1000</v>
       </c>
@@ -5124,7 +5242,7 @@
         <v>2099</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <f>A3+100</f>
         <v>1100</v>
@@ -5145,7 +5263,7 @@
         <v>2199</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A7" si="3">A4+100</f>
         <v>1200</v>
@@ -5166,7 +5284,7 @@
         <v>2299</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <f t="shared" si="3"/>
         <v>1300</v>
@@ -5187,7 +5305,7 @@
         <v>2399</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <f t="shared" si="3"/>
         <v>1400</v>
@@ -5207,18 +5325,18 @@
         <v>2999</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>75</v>
       </c>
       <c r="K9" t="s">
         <v>76</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -5262,23 +5380,24 @@
       <c r="Q10" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="R10" s="6"/>
+      <c r="U10" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>1000</v>
       </c>
@@ -5318,23 +5437,23 @@
       <c r="Q11" t="s">
         <v>73</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="U11" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="U11" t="s">
+      <c r="V11" t="s">
         <v>80</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="W11" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>1100</v>
       </c>
@@ -5374,23 +5493,23 @@
       <c r="Q12" t="s">
         <v>141</v>
       </c>
-      <c r="T12">
-        <v>1</v>
-      </c>
-      <c r="U12" t="s">
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
         <v>129</v>
       </c>
-      <c r="V12" t="s">
+      <c r="W12" t="s">
         <v>130</v>
       </c>
-      <c r="W12" t="s">
+      <c r="X12" t="s">
         <v>131</v>
       </c>
-      <c r="X12" t="s">
+      <c r="Y12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <f t="shared" ref="A13:A15" si="4">A12+100</f>
         <v>1200</v>
@@ -5432,7 +5551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <f t="shared" si="4"/>
         <v>1300</v>
@@ -5468,7 +5587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <f t="shared" si="4"/>
         <v>1400</v>
@@ -5486,11 +5605,11 @@
       <c r="H15" s="1"/>
       <c r="I15"/>
       <c r="K15" s="1"/>
-      <c r="T15" t="s">
+      <c r="U15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -5510,20 +5629,20 @@
       <c r="H16" s="1"/>
       <c r="I16"/>
       <c r="K16" s="1"/>
-      <c r="T16" t="s">
+      <c r="U16" t="s">
         <v>51</v>
       </c>
-      <c r="U16" t="s">
+      <c r="V16" t="s">
         <v>70</v>
       </c>
-      <c r="V16" t="s">
+      <c r="W16" t="s">
         <v>147</v>
       </c>
-      <c r="W16" t="s">
+      <c r="X16" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>2100</v>
       </c>
@@ -5542,26 +5661,26 @@
       <c r="G17"/>
       <c r="H17" s="1"/>
       <c r="I17"/>
-      <c r="T17">
-        <v>1</v>
-      </c>
       <c r="U17">
         <v>1</v>
       </c>
-      <c r="V17" t="s">
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
         <v>155</v>
       </c>
-      <c r="W17" t="s">
+      <c r="X17" t="s">
         <v>149</v>
       </c>
-      <c r="X17">
-        <v>0</v>
-      </c>
-      <c r="Y17" t="s">
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>2200</v>
       </c>
@@ -5580,14 +5699,14 @@
       <c r="G18"/>
       <c r="H18" s="1"/>
       <c r="I18"/>
-      <c r="X18">
-        <v>1</v>
-      </c>
-      <c r="Y18" t="s">
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>2300</v>
       </c>
@@ -5606,14 +5725,14 @@
       <c r="G19"/>
       <c r="H19" s="1"/>
       <c r="I19"/>
-      <c r="X19">
+      <c r="Y19">
         <v>2</v>
       </c>
-      <c r="Y19" t="s">
+      <c r="Z19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>2400</v>
       </c>
@@ -5633,22 +5752,28 @@
       <c r="H20" s="1"/>
       <c r="I20"/>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.15">
       <c r="G21"/>
       <c r="H21" s="1"/>
       <c r="I21"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="G25" s="1" t="s">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E25" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" t="s">
+        <v>305</v>
+      </c>
       <c r="G26" s="1" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>88</v>
@@ -5680,30 +5805,33 @@
       <c r="Q26" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="S26" t="s">
+      <c r="R26" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="T26" t="s">
         <v>51</v>
       </c>
-      <c r="T26" t="s">
+      <c r="U26" t="s">
         <v>112</v>
       </c>
-      <c r="U26" t="s">
+      <c r="V26" t="s">
         <v>113</v>
       </c>
-      <c r="V26" t="s">
+      <c r="W26" t="s">
         <v>114</v>
       </c>
-      <c r="W26" t="s">
+      <c r="X26" t="s">
         <v>115</v>
       </c>
-      <c r="X26" t="s">
+      <c r="Y26" t="s">
         <v>116</v>
       </c>
-      <c r="Y26" t="s">
+      <c r="Z26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="G27" s="1" t="s">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E27" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H27" s="1" t="s">
@@ -5736,10 +5864,17 @@
       <c r="Q27" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="G28" s="1">
+      <c r="R27" s="6"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E28" s="1">
         <v>10000</v>
+      </c>
+      <c r="F28" t="s">
+        <v>306</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>307</v>
       </c>
       <c r="H28" s="1">
         <v>3</v>
@@ -5771,11 +5906,11 @@
       <c r="Q28" s="1">
         <v>0</v>
       </c>
-      <c r="S28">
-        <v>1</v>
+      <c r="R28" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="T28">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="U28">
         <v>100</v>
@@ -5792,10 +5927,19 @@
       <c r="Y28">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="G29" s="1">
+      <c r="Z28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.15">
+      <c r="E29" s="1">
         <v>10001</v>
+      </c>
+      <c r="F29" t="s">
+        <v>308</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>309</v>
       </c>
       <c r="H29" s="1">
         <v>6</v>
@@ -5827,128 +5971,201 @@
       <c r="Q29" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="7:27" x14ac:dyDescent="0.15">
+      <c r="R29" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="33" spans="7:28" x14ac:dyDescent="0.15">
       <c r="G33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H33" t="s">
         <v>98</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="34" spans="7:27" x14ac:dyDescent="0.15">
+    <row r="34" spans="7:28" x14ac:dyDescent="0.15">
       <c r="H34" t="s">
         <v>99</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>51</v>
       </c>
-      <c r="T34" t="s">
+      <c r="U34" t="s">
         <v>65</v>
       </c>
-      <c r="U34" t="s">
+      <c r="V34" t="s">
         <v>128</v>
       </c>
-      <c r="V34" t="s">
+      <c r="W34" t="s">
         <v>70</v>
       </c>
-      <c r="W34" t="s">
+      <c r="X34" t="s">
         <v>159</v>
       </c>
-      <c r="X34" t="s">
+      <c r="Y34" t="s">
         <v>160</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AA34" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="S35" s="1">
-        <v>1</v>
-      </c>
-      <c r="T35" s="1" t="s">
+    <row r="35" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="T35" s="1">
+        <v>1</v>
+      </c>
+      <c r="U35" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="U35" t="s">
+      <c r="V35" t="s">
         <v>157</v>
       </c>
-      <c r="V35" s="1">
-        <v>0</v>
-      </c>
-      <c r="W35">
-        <v>0</v>
-      </c>
-      <c r="X35" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z35">
-        <v>0</v>
-      </c>
-      <c r="AA35" t="s">
+      <c r="W35" s="1">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="S36" s="1">
+    <row r="36" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="T36" s="1">
         <v>2</v>
       </c>
-      <c r="T36" s="1" t="s">
+      <c r="U36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="U36" t="s">
+      <c r="V36" t="s">
         <v>158</v>
       </c>
-      <c r="V36" s="1">
-        <v>1</v>
-      </c>
-      <c r="W36">
+      <c r="W36" s="1">
+        <v>1</v>
+      </c>
+      <c r="X36">
         <v>10000</v>
       </c>
-      <c r="X36" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z36">
-        <v>1</v>
-      </c>
-      <c r="AA36" t="s">
+      <c r="Y36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="Z37">
+    <row r="37" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="AA37">
         <v>2</v>
       </c>
-      <c r="AA37" t="s">
+      <c r="AB37" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="S40" t="s">
+    <row r="38" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="G38" s="1" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="39" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="G39" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="40" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="I40" s="6">
+        <v>-2000</v>
+      </c>
+      <c r="J40" s="6">
+        <v>0</v>
+      </c>
+      <c r="K40" s="6">
+        <v>1000</v>
+      </c>
+      <c r="L40" s="6">
+        <v>1000</v>
+      </c>
+      <c r="M40" s="6">
+        <v>0</v>
+      </c>
+      <c r="T40" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="41" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="S41" t="s">
+    <row r="41" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="G41" s="1">
+        <v>2</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="I41" s="6">
+        <v>0</v>
+      </c>
+      <c r="J41" s="6">
+        <v>0</v>
+      </c>
+      <c r="K41" s="6">
+        <v>0</v>
+      </c>
+      <c r="L41" s="6">
+        <v>0</v>
+      </c>
+      <c r="M41" s="6">
+        <v>3000</v>
+      </c>
+      <c r="T41" t="s">
         <v>51</v>
       </c>
-      <c r="T41" t="s">
+      <c r="U41" t="s">
         <v>152</v>
       </c>
-      <c r="U41" t="s">
+      <c r="V41" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="7:27" x14ac:dyDescent="0.15">
-      <c r="S42">
-        <v>1</v>
-      </c>
-      <c r="T42" t="s">
+    <row r="42" spans="7:28" x14ac:dyDescent="0.15">
+      <c r="T42">
+        <v>1</v>
+      </c>
+      <c r="U42" t="s">
         <v>153</v>
       </c>
-      <c r="U42" t="s">
+      <c r="V42" t="s">
         <v>154</v>
       </c>
     </row>
@@ -5966,7 +6183,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L58"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#Item Sprite #Hotkey show
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oas/Documents/work/github/newworld/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cn_Sky/newworld/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36880" yWindow="1740" windowWidth="35320" windowHeight="19880" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="2800" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
-    <sheet name="存储信息表" sheetId="8" r:id="rId2"/>
-    <sheet name="map" sheetId="3" r:id="rId3"/>
-    <sheet name="地理位置表" sheetId="7" r:id="rId4"/>
-    <sheet name="工作表1" sheetId="4" r:id="rId5"/>
+    <sheet name="map" sheetId="3" r:id="rId2"/>
+    <sheet name="地理位置表" sheetId="7" r:id="rId3"/>
+    <sheet name="工作表1" sheetId="4" r:id="rId4"/>
+    <sheet name="技能" sheetId="8" r:id="rId5"/>
     <sheet name="计划任务表" sheetId="5" r:id="rId6"/>
     <sheet name="备注表" sheetId="6" r:id="rId7"/>
     <sheet name="Items" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="340">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -1034,16 +1031,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>技能表</t>
-    <rPh sb="0" eb="1">
-      <t>ji'neng</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>biao</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>npc模板表</t>
     <rPh sb="3" eb="4">
       <t>mu'ban</t>
@@ -1058,20 +1045,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>心法</t>
-    <rPh sb="0" eb="1">
-      <t>xin'fa</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>防御</t>
-    <rPh sb="0" eb="1">
-      <t>fang'yu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>10000|一个疯和尚不由分说朝你杀来。</t>
     <rPh sb="6" eb="7">
       <t>yi'ge</t>
@@ -1105,26 +1078,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>紫霞功</t>
-    <rPh sb="0" eb="1">
-      <t>zi'xia</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>gong</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>紫霞指</t>
-    <rPh sb="0" eb="1">
-      <t>zi'xia</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>zhi'fa</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>条件文本</t>
     <rPh sb="0" eb="1">
       <t>tiao'jian</t>
@@ -1255,18 +1208,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>一指出，万人屠。</t>
-    <rPh sb="4" eb="5">
-      <t>wan'ren'tu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>power</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>effectId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2826,126 +2768,199 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>地图开放数据</t>
-    <rPh sb="0" eb="1">
-      <t>di'tu</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>kai'fang</t>
+    <t>灭神咒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语出，神灭。</t>
+    <rPh sb="0" eb="1">
+      <t>yu'chu</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>shen'mie</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>指尖所向，万物虚无。</t>
+    <rPh sb="5" eb="6">
+      <t>wan'wu</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>xu'wu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cd</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吟唱时间</t>
+    <rPh sb="0" eb="1">
+      <t>yin'chang</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>shi'jian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>costType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消耗类型</t>
+    <rPh sb="0" eb="1">
+      <t>xiao'hao</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>lei'xing</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>costValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>powerInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害成长</t>
+    <rPh sb="0" eb="1">
+      <t>shang'hai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>cheng'zhang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫霞拳</t>
+    <rPh sb="0" eb="1">
+      <t>zi'xia</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>quan'fa</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紫霞仙人指</t>
+    <rPh sb="0" eb="1">
+      <t>zi'xia</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>xian'ren</t>
     </rPh>
     <rPh sb="4" eb="5">
-      <t>shu'ju</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>当前地图数据</t>
-    <rPh sb="0" eb="1">
-      <t>dang'qian</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>di'tu</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>shu'ju</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC成长数据</t>
-    <rPh sb="3" eb="4">
-      <t>cheng'zhang</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>shu'ju</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>存活年限？？</t>
-    <rPh sb="0" eb="1">
-      <t>cun'huo</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>nian'xian</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>可根据悟性、缘分、灵根等计算出最大存活年限，并根据随机事件判断具体死亡时期。</t>
-    <rPh sb="0" eb="1">
-      <t>ke</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>gen'ju</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>wu'xing</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>yuan'fen</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>ling'gen</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>deng</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>ji'suan'chu</t>
-    </rPh>
-    <rPh sb="15" eb="16">
-      <t>zui'da</t>
-    </rPh>
-    <rPh sb="17" eb="18">
-      <t>cun'huo</t>
-    </rPh>
-    <rPh sb="19" eb="20">
-      <t>nian'xian</t>
-    </rPh>
-    <rPh sb="22" eb="23">
-      <t>bing</t>
-    </rPh>
-    <rPh sb="23" eb="24">
-      <t>gen'ju</t>
-    </rPh>
-    <rPh sb="25" eb="26">
-      <t>sui'ji</t>
-    </rPh>
-    <rPh sb="27" eb="28">
-      <t>shi'jian</t>
-    </rPh>
-    <rPh sb="29" eb="30">
-      <t>pan'duan</t>
-    </rPh>
-    <rPh sb="31" eb="32">
-      <t>ju'ti</t>
-    </rPh>
-    <rPh sb="33" eb="34">
-      <t>si'wang</t>
-    </rPh>
-    <rPh sb="35" eb="36">
-      <t>shi'qi</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NPC属性增加出生时期、派别</t>
-    <rPh sb="3" eb="4">
-      <t>shu'xing</t>
-    </rPh>
-    <rPh sb="5" eb="6">
-      <t>zeng'jia</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>chu'sheng</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>shi'qi</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>pai'bie</t>
-    </rPh>
+      <t>zhi'fa</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Mental,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF888A85"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>//心法</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>PhysicalAttack,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF888A85"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>//肉体攻击</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MagicalAttack,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF888A85"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>//法力攻击</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>SoulAttack,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF888A85"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>//灵魂攻击</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddShield,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AddBuff,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0Strength</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Mp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2Hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3Spirit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4MaxHp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5MaxAge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffParam</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buffParamInc</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2953,7 +2968,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2968,6 +2983,16 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Menlo"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF888A85"/>
+      <name val="Menlo"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2990,7 +3015,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3013,6 +3038,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3303,7 +3332,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3327,7 +3356,7 @@
         <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -3425,13 +3454,13 @@
         <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
@@ -3445,40 +3474,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
@@ -3530,7 +3525,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3580,60 +3575,60 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="K7" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="L7" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="S7" t="s">
         <v>265</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>282</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="S7" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5">
@@ -3669,18 +3664,18 @@
         <v>20</v>
       </c>
       <c r="S8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="T8" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="U8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -3718,21 +3713,21 @@
         <v>20,30</v>
       </c>
       <c r="S9" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="T9" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="U9" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="V9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -3770,18 +3765,18 @@
         <v>20,30,50</v>
       </c>
       <c r="T10" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="U10" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="V10" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -3821,18 +3816,18 @@
         <v>20,30,50,40</v>
       </c>
       <c r="T11" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="U11" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="V11" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5">
@@ -3866,12 +3861,12 @@
         <v>20,30,50,40,40</v>
       </c>
       <c r="V12" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3909,15 +3904,15 @@
         <v>20,30,50,40,40,30</v>
       </c>
       <c r="T13" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="U13" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -3955,7 +3950,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4487,20 +4482,20 @@
     </row>
     <row r="28" spans="2:21" x14ac:dyDescent="0.15">
       <c r="S28" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="U28" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U29" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U30" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="2:21" x14ac:dyDescent="0.15">
@@ -4510,17 +4505,17 @@
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.15">
       <c r="U32" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U33" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="34" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U34" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -4529,7 +4524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CW101"/>
   <sheetViews>
@@ -5349,12 +5344,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB42"/>
+  <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView topLeftCell="N15" workbookViewId="0">
+      <selection activeCell="T33" sqref="T33:AB37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -5371,14 +5366,14 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="D2" s="7" t="s">
+      <c r="B2" s="8"/>
+      <c r="D2" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
@@ -5649,7 +5644,7 @@
         <v>83</v>
       </c>
       <c r="Q12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="U12">
         <v>1</v>
@@ -5697,7 +5692,7 @@
         <v>1</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O13" s="1">
         <v>2</v>
@@ -5739,7 +5734,7 @@
         <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="Q14" t="s">
         <v>86</v>
@@ -5764,7 +5759,7 @@
       <c r="I15"/>
       <c r="K15" s="1"/>
       <c r="U15" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.15">
@@ -5794,10 +5789,10 @@
         <v>70</v>
       </c>
       <c r="W16" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="X16" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.15">
@@ -5826,10 +5821,10 @@
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="X17" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -5861,7 +5856,7 @@
         <v>1</v>
       </c>
       <c r="Z18" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.15">
@@ -5869,7 +5864,7 @@
         <v>2300</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C19" s="1">
         <v>4</v>
@@ -5895,7 +5890,7 @@
         <v>2400</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C20" s="1">
         <v>5</v>
@@ -5920,7 +5915,7 @@
         <v>87</v>
       </c>
       <c r="T25" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.15">
@@ -5928,7 +5923,7 @@
         <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>128</v>
@@ -5943,7 +5938,7 @@
         <v>90</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>96</v>
@@ -5964,7 +5959,7 @@
         <v>107</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="T26" t="s">
         <v>51</v>
@@ -6029,10 +6024,10 @@
         <v>10000</v>
       </c>
       <c r="F28" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="H28" s="1">
         <v>3</v>
@@ -6053,7 +6048,7 @@
         <v>1</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O28" s="1">
         <v>2</v>
@@ -6065,7 +6060,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="T28">
         <v>1</v>
@@ -6094,10 +6089,10 @@
         <v>10001</v>
       </c>
       <c r="F29" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="H29" s="1">
         <v>6</v>
@@ -6118,7 +6113,7 @@
         <v>2</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O29" s="1">
         <v>0</v>
@@ -6130,153 +6125,56 @@
         <v>0</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="M31" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.15">
-      <c r="M32" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="33" spans="7:28" x14ac:dyDescent="0.15">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="33" spans="7:22" x14ac:dyDescent="0.15">
       <c r="G33" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H33" t="s">
         <v>98</v>
       </c>
-      <c r="M33" t="s">
-        <v>324</v>
-      </c>
-      <c r="T33" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="7:28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="34" spans="7:22" x14ac:dyDescent="0.15">
       <c r="H34" t="s">
         <v>99</v>
       </c>
-      <c r="T34" t="s">
-        <v>51</v>
-      </c>
-      <c r="U34" t="s">
-        <v>65</v>
-      </c>
-      <c r="V34" t="s">
-        <v>128</v>
-      </c>
-      <c r="W34" t="s">
-        <v>70</v>
-      </c>
-      <c r="X34" t="s">
-        <v>159</v>
-      </c>
-      <c r="Y34" t="s">
-        <v>160</v>
-      </c>
-      <c r="AA34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="7:28" x14ac:dyDescent="0.15">
-      <c r="T35" s="1">
-        <v>1</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="V35" t="s">
-        <v>157</v>
-      </c>
-      <c r="W35" s="1">
-        <v>0</v>
-      </c>
-      <c r="X35">
-        <v>0</v>
-      </c>
-      <c r="Y35" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA35">
-        <v>0</v>
-      </c>
-      <c r="AB35" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="36" spans="7:28" x14ac:dyDescent="0.15">
-      <c r="T36" s="1">
-        <v>2</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="V36" t="s">
-        <v>158</v>
-      </c>
-      <c r="W36" s="1">
-        <v>1</v>
-      </c>
-      <c r="X36">
-        <v>10000</v>
-      </c>
-      <c r="Y36" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA36">
-        <v>1</v>
-      </c>
-      <c r="AB36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="7:28" x14ac:dyDescent="0.15">
-      <c r="AA37">
-        <v>2</v>
-      </c>
-      <c r="AB37" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="7:28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="38" spans="7:22" x14ac:dyDescent="0.15">
       <c r="G38" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="7:22" x14ac:dyDescent="0.15">
+      <c r="G39" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="39" spans="7:28" x14ac:dyDescent="0.15">
-      <c r="G39" s="1" t="s">
+      <c r="J39" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="K39" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="H39" s="6" t="s">
+      <c r="L39" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="J39" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="K39" s="6" t="s">
+      <c r="M39" s="6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="40" spans="7:22" x14ac:dyDescent="0.15">
+      <c r="G40" s="1">
+        <v>1</v>
+      </c>
+      <c r="H40" s="6" t="s">
         <v>311</v>
-      </c>
-      <c r="L39" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="40" spans="7:28" x14ac:dyDescent="0.15">
-      <c r="G40" s="1">
-        <v>1</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="I40" s="6">
         <v>-2000</v>
@@ -6294,15 +6192,15 @@
         <v>0</v>
       </c>
       <c r="T40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="7:28" x14ac:dyDescent="0.15">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="41" spans="7:22" x14ac:dyDescent="0.15">
       <c r="G41" s="1">
         <v>2</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="I41" s="6">
         <v>0</v>
@@ -6323,21 +6221,21 @@
         <v>51</v>
       </c>
       <c r="U41" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="V41" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="42" spans="7:28" x14ac:dyDescent="0.15">
+    <row r="42" spans="7:22" x14ac:dyDescent="0.15">
       <c r="T42">
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="V42" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -6345,6 +6243,238 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" t="s">
+        <v>314</v>
+      </c>
+      <c r="F1" t="s">
+        <v>316</v>
+      </c>
+      <c r="G1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H1" t="s">
+        <v>320</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
+        <v>321</v>
+      </c>
+      <c r="K1" t="s">
+        <v>337</v>
+      </c>
+      <c r="L1" t="s">
+        <v>338</v>
+      </c>
+      <c r="M1" t="s">
+        <v>339</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="R1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>317</v>
+      </c>
+      <c r="G2" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" t="s">
+        <v>322</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="R2" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7">
+        <v>20</v>
+      </c>
+      <c r="I3" s="7">
+        <v>500</v>
+      </c>
+      <c r="J3" s="7">
+        <v>50</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="R3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="7">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>30</v>
+      </c>
+      <c r="I4" s="7">
+        <v>800</v>
+      </c>
+      <c r="J4" s="7">
+        <v>80</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>328</v>
+      </c>
+      <c r="R4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>2</v>
+      </c>
+      <c r="I5" s="7">
+        <v>400</v>
+      </c>
+      <c r="J5" s="7">
+        <v>50</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="R5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+      <c r="O6" s="9" t="s">
+        <v>330</v>
+      </c>
+      <c r="R6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6369,166 +6499,166 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
       </c>
       <c r="J2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="K2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="L2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="J3" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E4" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="F4" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="F5" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="F6" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="F7" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F8" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="F10" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="F11" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G11" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="H11" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F12" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="G12" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="H12" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F13" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="G13" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="B18" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
@@ -6536,178 +6666,178 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="B37" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B44" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B46" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B48" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B49" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B51" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C53" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C54" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="B56" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B57" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
   </sheetData>
@@ -6736,53 +6866,53 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C4" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Add skill handler #redo battle unit and battle unit info #change skill design #plan to add different shield
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28130"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cn_Sky/newworld/Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oas/Documents/work/github/newworld/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="460" windowWidth="24600" windowHeight="15540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="2640" yWindow="1600" windowWidth="32500" windowHeight="18700" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="350">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -2879,34 +2882,6 @@
   </si>
   <si>
     <r>
-      <t>PhysicalAttack,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF888A85"/>
-        <rFont val="Menlo"/>
-      </rPr>
-      <t>//肉体攻击</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>MagicalAttack,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF888A85"/>
-        <rFont val="Menlo"/>
-      </rPr>
-      <t>//法力攻击</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
       <t>SoulAttack,</t>
     </r>
     <r>
@@ -2924,10 +2899,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>AddBuff,</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0Strength</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2944,10 +2915,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4MaxHp</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>5MaxAge</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2961,6 +2928,201 @@
   </si>
   <si>
     <t>buffParamInc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加nextLevelId</t>
+    <rPh sb="0" eb="1">
+      <t>zeng'jia</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加newSKillId</t>
+    <rPh sb="0" eb="1">
+      <t>zeng'jai</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>升级后的技能</t>
+    <rPh sb="0" eb="1">
+      <t>sheng'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>hou</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>d</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ji'neng</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>心法类技能升级后，开放新技能</t>
+    <rPh sb="0" eb="1">
+      <t>xin'fa'lei</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>lei</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ji'neng</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>sheng'ji'hou</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>kai'fang</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>xin'ji'neng</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//斩杀</t>
+    <rPh sb="2" eb="3">
+      <t>zhan'sha</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>法力流失</t>
+    <rPh sb="0" eb="1">
+      <t>fa'li</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>liu'shi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逼毒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StrengthAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>MpAttack,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF888A85"/>
+        <rFont val="Menlo"/>
+      </rPr>
+      <t>//肉体攻击</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuckMp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuckMaxMp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>需要有释放限制，且会影响战斗外属性</t>
+    <rPh sb="0" eb="1">
+      <t>xu'yao</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>you</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>shi'fang</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>xian'zhi</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>qie</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>hui</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ying'xiang</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>zhan'dou</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>wai</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>shu'xing</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加元素亲和度，亲和力越高，施法速度加快，威力提高</t>
+    <rPh sb="0" eb="1">
+      <t>zeng'jai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>yuan'su</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>qin'he'du</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>qin'he'li</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>yue'gao</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>shi'fa</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>su'du</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>jia'kuai</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>wei'li</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ti'gao</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>增加护盾种类，护盾和攻击有生克关系</t>
+    <rPh sb="0" eb="1">
+      <t>zeng'jia</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>hu'dun</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>zhong'lei</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>hu'dun</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>he</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>you</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>sheng'ke'guan'xi</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3038,10 +3200,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -5366,14 +5528,14 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="D2" s="8" t="s">
+      <c r="B2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
@@ -6250,18 +6412,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R6"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -6293,22 +6456,22 @@
         <v>321</v>
       </c>
       <c r="K1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="L1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="M1" t="s">
-        <v>339</v>
-      </c>
-      <c r="O1" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="O1" s="8" t="s">
         <v>325</v>
       </c>
       <c r="R1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
         <v>317</v>
       </c>
@@ -6318,14 +6481,14 @@
       <c r="J2" t="s">
         <v>322</v>
       </c>
-      <c r="O2" s="9" t="s">
-        <v>326</v>
+      <c r="O2" t="s">
+        <v>343</v>
       </c>
       <c r="R2" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
@@ -6365,14 +6528,14 @@
       <c r="M3" s="7">
         <v>0</v>
       </c>
-      <c r="O3" s="9" t="s">
-        <v>327</v>
+      <c r="O3" s="8" t="s">
+        <v>344</v>
       </c>
       <c r="R3" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
@@ -6412,14 +6575,20 @@
       <c r="M4" s="7">
         <v>0</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>328</v>
+      <c r="O4" s="8" t="s">
+        <v>326</v>
       </c>
       <c r="R4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+      <c r="T4" t="s">
+        <v>336</v>
+      </c>
+      <c r="U4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -6459,19 +6628,51 @@
       <c r="M5" s="7">
         <v>0</v>
       </c>
-      <c r="O5" s="9" t="s">
-        <v>329</v>
+      <c r="O5" s="8" t="s">
+        <v>327</v>
       </c>
       <c r="R5" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="O6" s="9" t="s">
-        <v>330</v>
-      </c>
-      <c r="R6" t="s">
-        <v>336</v>
+        <v>332</v>
+      </c>
+      <c r="T5" t="s">
+        <v>337</v>
+      </c>
+      <c r="U5" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O6" s="8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O7" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="P7" t="s">
+        <v>347</v>
+      </c>
+      <c r="T7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="O8" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="T8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="R9" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="R10" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Battle Debug #Battle Flow
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1600" windowWidth="32500" windowHeight="18700" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="355">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -2828,20 +2828,6 @@
   </si>
   <si>
     <t>costValue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>powerInc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>伤害成长</t>
-    <rPh sb="0" eb="1">
-      <t>shang'hai</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>cheng'zhang</t>
-    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3123,6 +3109,55 @@
     <rPh sb="13" eb="14">
       <t>sheng'ke'guan'xi</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>powerFixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>固定伤害</t>
+    <rPh sb="0" eb="1">
+      <t>gu'ding</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>shang'hai</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>伤害比例</t>
+    <rPh sb="0" eb="1">
+      <t>shang'hai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>bi'li</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>buff类型</t>
+    <rPh sb="4" eb="5">
+      <t>lei'xing</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Range</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击范围</t>
+    <rPh sb="0" eb="1">
+      <t>gong'ji</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>fan'wei</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprite</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3177,7 +3212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3201,6 +3236,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5528,14 +5566,14 @@
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="10"/>
+      <c r="D2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
@@ -6412,19 +6450,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U10"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>51</v>
       </c>
@@ -6453,47 +6491,68 @@
         <v>153</v>
       </c>
       <c r="J1" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="K1" t="s">
+        <v>331</v>
+      </c>
+      <c r="L1" t="s">
+        <v>332</v>
+      </c>
+      <c r="M1" t="s">
         <v>333</v>
       </c>
-      <c r="L1" t="s">
-        <v>334</v>
-      </c>
-      <c r="M1" t="s">
-        <v>335</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="R1" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="N1" t="s">
+        <v>352</v>
+      </c>
+      <c r="O1" t="s">
+        <v>354</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="T1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
         <v>317</v>
       </c>
       <c r="G2" t="s">
         <v>319</v>
       </c>
+      <c r="I2" t="s">
+        <v>350</v>
+      </c>
       <c r="J2" t="s">
-        <v>322</v>
+        <v>349</v>
+      </c>
+      <c r="K2" t="s">
+        <v>351</v>
+      </c>
+      <c r="L2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N2" t="s">
+        <v>353</v>
       </c>
       <c r="O2" t="s">
-        <v>343</v>
-      </c>
-      <c r="R2" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>341</v>
+      </c>
+      <c r="T2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>152</v>
@@ -6528,19 +6587,25 @@
       <c r="M3" s="7">
         <v>0</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="R3" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+      <c r="N3" s="9">
+        <v>5</v>
+      </c>
+      <c r="O3" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="T3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>315</v>
@@ -6575,20 +6640,26 @@
       <c r="M4" s="7">
         <v>0</v>
       </c>
-      <c r="O4" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="R4" t="s">
-        <v>331</v>
+      <c r="N4" s="9">
+        <v>20</v>
+      </c>
+      <c r="O4" s="9">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>324</v>
       </c>
       <c r="T4" t="s">
+        <v>329</v>
+      </c>
+      <c r="V4" t="s">
+        <v>334</v>
+      </c>
+      <c r="W4" t="s">
         <v>336</v>
       </c>
-      <c r="U4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>3</v>
       </c>
@@ -6628,51 +6699,57 @@
       <c r="M5" s="7">
         <v>0</v>
       </c>
-      <c r="O5" s="8" t="s">
-        <v>327</v>
-      </c>
-      <c r="R5" t="s">
-        <v>332</v>
+      <c r="N5" s="9">
+        <v>80</v>
+      </c>
+      <c r="O5" s="9">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>325</v>
       </c>
       <c r="T5" t="s">
+        <v>330</v>
+      </c>
+      <c r="V5" t="s">
+        <v>335</v>
+      </c>
+      <c r="W5" t="s">
         <v>337</v>
       </c>
-      <c r="U5" t="s">
+    </row>
+    <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q6" s="8" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q7" s="8" t="s">
+        <v>344</v>
+      </c>
+      <c r="R7" t="s">
+        <v>345</v>
+      </c>
+      <c r="V7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="Q8" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="V8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="T9" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="O6" s="8" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="O7" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="P7" t="s">
-        <v>347</v>
-      </c>
-      <c r="T7" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" ht="16" x14ac:dyDescent="0.2">
-      <c r="O8" s="8" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="T10" t="s">
         <v>340</v>
-      </c>
-      <c r="T8" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="R9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="R10" t="s">
-        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Add Dialogue #Debug Mist #Link npc to battle
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="360">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -1158,38 +1158,6 @@
   </si>
   <si>
     <t>questions</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>敢问大师法号？|大师给我算一卦。</t>
-    <rPh sb="8" eb="9">
-      <t>da'shi</t>
-    </rPh>
-    <rPh sb="10" eb="11">
-      <t>gei</t>
-    </rPh>
-    <rPh sb="11" eb="12">
-      <t>wo</t>
-    </rPh>
-    <rPh sb="12" eb="13">
-      <t>suan'yi'gua</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>贫僧法号星云。|天机不可泄露。</t>
-    <rPh sb="0" eb="1">
-      <t>pin'seng</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>fa'hao</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>xing'yun</t>
-    </rPh>
-    <rPh sb="8" eb="9">
-      <t>tian'ji'bu'ke'xi</t>
-    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -3182,6 +3150,76 @@
   </si>
   <si>
     <t>Npc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>actions</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>施主此来有何贵干？|敢问大师法号？|大师给我算一卦。|大师，老子想揍你！</t>
+    <rPh sb="0" eb="1">
+      <t>shi'zhu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ci</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>you'he'gui'gan</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>da'shi</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>gei</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>wo</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>suan'yi'gua</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>da'shi</t>
+    </rPh>
+    <rPh sb="30" eb="31">
+      <t>lao'zi</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>xiang'zou'ni</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贫僧法号星云。|天机不可泄露。|拳脚无眼，施主小心了！</t>
+    <rPh sb="0" eb="1">
+      <t>pin'seng</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>fa'hao</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>xing'yun</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>tian'ji'bu'ke'xi</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>quan'jiao'wu'yan</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shi'zhu</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>xiao'xin</t>
+    </rPh>
+    <rPh sb="25" eb="26">
+      <t>l</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0|0|1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3556,7 +3594,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3580,7 +3618,7 @@
         <v>104</v>
       </c>
       <c r="I1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.15">
@@ -3678,13 +3716,13 @@
         <v>104</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2" t="s">
@@ -3701,7 +3739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -3749,7 +3787,7 @@
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -3799,60 +3837,60 @@
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>250</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F7" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>258</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="I7" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>273</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="J7" s="5" t="s">
+      <c r="P7" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="S7" t="s">
         <v>263</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="L7" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="N7" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="O7" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="P7" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="S7" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5">
@@ -3888,18 +3926,18 @@
         <v>20</v>
       </c>
       <c r="S8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="T8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="U8" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
@@ -3937,21 +3975,21 @@
         <v>20,30</v>
       </c>
       <c r="S9" t="s">
+        <v>270</v>
+      </c>
+      <c r="T9" t="s">
         <v>272</v>
       </c>
-      <c r="T9" t="s">
-        <v>274</v>
-      </c>
       <c r="U9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="V9" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -3989,18 +4027,18 @@
         <v>20,30,50</v>
       </c>
       <c r="T10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="U10" t="s">
+        <v>285</v>
+      </c>
+      <c r="V10" t="s">
         <v>287</v>
-      </c>
-      <c r="V10" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -4040,18 +4078,18 @@
         <v>20,30,50,40</v>
       </c>
       <c r="T11" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="U11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="V11" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5">
@@ -4085,12 +4123,12 @@
         <v>20,30,50,40,40</v>
       </c>
       <c r="V12" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -4128,15 +4166,15 @@
         <v>20,30,50,40,40,30</v>
       </c>
       <c r="T13" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="U13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -4174,7 +4212,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -4706,31 +4744,31 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="S28" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="U28" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="U29" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
       <c r="U30" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.15">
@@ -4740,17 +4778,17 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.15">
       <c r="U32" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="33" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U33" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="21:21" x14ac:dyDescent="0.15">
       <c r="U34" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5583,8 +5621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView topLeftCell="N15" workbookViewId="0">
-      <selection activeCell="T33" sqref="T33:AB37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -6027,7 +6065,7 @@
         <v>142</v>
       </c>
       <c r="X16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.15">
@@ -6056,7 +6094,7 @@
         <v>1</v>
       </c>
       <c r="W17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="X17" t="s">
         <v>144</v>
@@ -6158,7 +6196,7 @@
         <v>51</v>
       </c>
       <c r="F26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>128</v>
@@ -6173,7 +6211,7 @@
         <v>90</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>96</v>
@@ -6194,7 +6232,7 @@
         <v>107</v>
       </c>
       <c r="R26" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="T26" t="s">
         <v>51</v>
@@ -6259,10 +6297,10 @@
         <v>10000</v>
       </c>
       <c r="F28" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H28" s="1">
         <v>3</v>
@@ -6295,7 +6333,7 @@
         <v>0</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="T28">
         <v>1</v>
@@ -6324,10 +6362,10 @@
         <v>10001</v>
       </c>
       <c r="F29" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="H29" s="1">
         <v>6</v>
@@ -6360,10 +6398,10 @@
         <v>0</v>
       </c>
       <c r="R29" s="6" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="33" spans="7:22" x14ac:dyDescent="0.15">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="33" spans="7:23" x14ac:dyDescent="0.15">
       <c r="G33" s="1" t="s">
         <v>97</v>
       </c>
@@ -6371,45 +6409,45 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="7:22" x14ac:dyDescent="0.15">
+    <row r="34" spans="7:23" x14ac:dyDescent="0.15">
       <c r="H34" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="38" spans="7:22" x14ac:dyDescent="0.15">
+    <row r="38" spans="7:23" x14ac:dyDescent="0.15">
       <c r="G38" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="39" spans="7:23" x14ac:dyDescent="0.15">
+      <c r="G39" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H39" s="6" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="39" spans="7:22" x14ac:dyDescent="0.15">
-      <c r="G39" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>298</v>
-      </c>
       <c r="I39" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="L39" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="J39" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="K39" s="6" t="s">
+      <c r="M39" s="6" t="s">
         <v>304</v>
       </c>
-      <c r="L39" s="6" t="s">
-        <v>305</v>
-      </c>
-      <c r="M39" s="6" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="40" spans="7:22" x14ac:dyDescent="0.15">
+    </row>
+    <row r="40" spans="7:23" x14ac:dyDescent="0.15">
       <c r="G40" s="1">
         <v>1</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I40" s="6">
         <v>-2000</v>
@@ -6430,12 +6468,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="41" spans="7:22" x14ac:dyDescent="0.15">
+    <row r="41" spans="7:23" x14ac:dyDescent="0.15">
       <c r="G41" s="1">
         <v>2</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="I41" s="6">
         <v>0</v>
@@ -6461,16 +6499,22 @@
       <c r="V41" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="42" spans="7:22" x14ac:dyDescent="0.15">
+      <c r="W41" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="42" spans="7:23" x14ac:dyDescent="0.15">
       <c r="T42">
         <v>1</v>
       </c>
       <c r="U42" t="s">
-        <v>148</v>
+        <v>357</v>
       </c>
       <c r="V42" t="s">
-        <v>149</v>
+        <v>358</v>
+      </c>
+      <c r="W42" t="s">
+        <v>359</v>
       </c>
     </row>
   </sheetData>
@@ -6511,75 +6555,75 @@
         <v>70</v>
       </c>
       <c r="E1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F1" t="s">
         <v>314</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>316</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>318</v>
       </c>
-      <c r="H1" t="s">
-        <v>320</v>
-      </c>
       <c r="I1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K1" t="s">
+        <v>329</v>
+      </c>
+      <c r="L1" t="s">
+        <v>330</v>
+      </c>
+      <c r="M1" t="s">
         <v>331</v>
       </c>
-      <c r="L1" t="s">
-        <v>332</v>
-      </c>
-      <c r="M1" t="s">
-        <v>333</v>
-      </c>
       <c r="N1" t="s">
+        <v>350</v>
+      </c>
+      <c r="O1" t="s">
         <v>352</v>
       </c>
-      <c r="O1" t="s">
-        <v>354</v>
-      </c>
       <c r="Q1" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="T1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" t="s">
         <v>317</v>
       </c>
-      <c r="G2" t="s">
-        <v>319</v>
-      </c>
       <c r="I2" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J2" t="s">
+        <v>347</v>
+      </c>
+      <c r="K2" t="s">
         <v>349</v>
-      </c>
-      <c r="K2" t="s">
-        <v>351</v>
       </c>
       <c r="L2" t="s">
         <v>81</v>
       </c>
       <c r="N2" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="O2" t="s">
         <v>71</v>
       </c>
       <c r="Q2" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="T2" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6587,10 +6631,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D3" s="1">
         <v>1</v>
@@ -6629,10 +6673,10 @@
         <v>1</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="T3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6640,10 +6684,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D4" s="1">
         <v>2</v>
@@ -6682,16 +6726,16 @@
         <v>2</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="T4" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="V4" t="s">
+        <v>332</v>
+      </c>
+      <c r="W4" t="s">
         <v>334</v>
-      </c>
-      <c r="W4" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="16" x14ac:dyDescent="0.2">
@@ -6699,10 +6743,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D5" s="7">
         <v>3</v>
@@ -6741,50 +6785,50 @@
         <v>3</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="T5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="V5" t="s">
+        <v>333</v>
+      </c>
+      <c r="W5" t="s">
         <v>335</v>
-      </c>
-      <c r="W5" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="Q6" s="8" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="Q7" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="R7" t="s">
+        <v>343</v>
+      </c>
+      <c r="V7" t="s">
         <v>344</v>
-      </c>
-      <c r="R7" t="s">
-        <v>345</v>
-      </c>
-      <c r="V7" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="Q8" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="V8" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.15">
       <c r="T9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="T10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -6812,166 +6856,166 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
         <v>99</v>
       </c>
       <c r="J2" t="s">
+        <v>224</v>
+      </c>
+      <c r="K2" t="s">
+        <v>225</v>
+      </c>
+      <c r="L2" t="s">
         <v>226</v>
-      </c>
-      <c r="K2" t="s">
-        <v>227</v>
-      </c>
-      <c r="L2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="E4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F7" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B9" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B11" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F11" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G11" t="s">
+        <v>217</v>
+      </c>
+      <c r="H11" t="s">
         <v>219</v>
-      </c>
-      <c r="H11" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B12" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="H12" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B13" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.15">
       <c r="B16" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B19" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B21" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.15">
@@ -6979,178 +7023,178 @@
         <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B25" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B27" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B29" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B32" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B33" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B34" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B37" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B39" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B40" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B41" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B42" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B43" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B45" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.15">
       <c r="B46" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B49" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B50" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B51" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
+        <v>221</v>
+      </c>
+      <c r="B53" t="s">
         <v>223</v>
       </c>
-      <c r="B53" t="s">
-        <v>225</v>
-      </c>
       <c r="C53" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B54" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C54" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B56" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B57" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B58" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -7179,53 +7223,53 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#Collect All #TreasureBox Done #Debug Inventory,BeiBao,QianKunDai #Add Test Treasure
</commit_message>
<xml_diff>
--- a/Design/new world.xlsx
+++ b/Design/new world.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="功能按钮" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="363">
   <si>
     <t>背包</t>
     <rPh sb="0" eb="1">
@@ -3220,6 +3220,57 @@
   </si>
   <si>
     <t>0|0|1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树木可以砍伐</t>
+    <rPh sb="0" eb="1">
+      <t>shu'mu</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>kan'fa</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石块可以挖掘</t>
+    <rPh sb="0" eb="1">
+      <t>shi'kuai</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>wa'jue</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>绝大部分内容都可以挖掘获取物品</t>
+    <rPh sb="0" eb="1">
+      <t>jue'da'bu'fen</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>nei'rong</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>dou</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ke'yi</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>wa'jue</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>huo'qu</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>wu'pin</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3739,8 +3790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -4751,6 +4802,9 @@
       <c r="A28" t="s">
         <v>354</v>
       </c>
+      <c r="F28" t="s">
+        <v>360</v>
+      </c>
       <c r="S28" t="s">
         <v>276</v>
       </c>
@@ -4762,11 +4816,17 @@
       <c r="A29" t="s">
         <v>355</v>
       </c>
+      <c r="F29" t="s">
+        <v>361</v>
+      </c>
       <c r="U29" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="F30" t="s">
+        <v>362</v>
+      </c>
       <c r="U30" t="s">
         <v>279</v>
       </c>
@@ -5621,7 +5681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>

</xml_diff>